<commit_message>
Intentos - Captura de pantalla
</commit_message>
<xml_diff>
--- a/PegaRobotic/Files/DatosExcel.xlsx
+++ b/PegaRobotic/Files/DatosExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PegaRobotic\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD5C814-9154-42BD-A5AF-AD747576FC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A494264F-5410-4E93-B04F-65C1F7FADC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -57,15 +57,9 @@
     <t>SEGUNDA PREGUNTA</t>
   </si>
   <si>
-    <t>tattthhhhQ@hh_</t>
-  </si>
-  <si>
     <t>es</t>
   </si>
   <si>
-    <t>Yulino123..</t>
-  </si>
-  <si>
     <t>apurimac</t>
   </si>
   <si>
@@ -75,10 +69,19 @@
     <t>B</t>
   </si>
   <si>
-    <t>tatttxxxxhQ@hh_</t>
-  </si>
-  <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Tata..QQ@2</t>
+  </si>
+  <si>
+    <t>yulino44</t>
+  </si>
+  <si>
+    <t>Peru$2023@@</t>
+  </si>
+  <si>
+    <t>jordan2023.</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,17 +130,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,14 +420,14 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
@@ -470,31 +471,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -502,38 +503,35 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{DC797EA4-55D4-4A93-A7FA-D91860FED67D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
logica en el script
</commit_message>
<xml_diff>
--- a/PegaRobotic/Files/DatosExcel.xlsx
+++ b/PegaRobotic/Files/DatosExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PegaRobotic\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A494264F-5410-4E93-B04F-65C1F7FADC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427748DC-DAB6-488D-9FC9-09C5FDC9332F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -39,56 +39,62 @@
     <t>PASSWORD 1</t>
   </si>
   <si>
+    <t>RESPUESTA 1</t>
+  </si>
+  <si>
+    <t>RESPUESTA 2</t>
+  </si>
+  <si>
+    <t>TIPO CUENTA</t>
+  </si>
+  <si>
+    <t>SEGUNDA PREGUNTA</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>apurimac</t>
+  </si>
+  <si>
+    <t>chocolate</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Tata..QQ@2</t>
+  </si>
+  <si>
+    <t>yulino44</t>
+  </si>
+  <si>
+    <t>Peru$2023@@</t>
+  </si>
+  <si>
+    <t>jordan2023.</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>MENSAJE</t>
+  </si>
+  <si>
     <t>PASSWORD 2</t>
   </si>
   <si>
-    <t>PRIMERA PREGUNTA</t>
-  </si>
-  <si>
-    <t>RESPUESTA 1</t>
-  </si>
-  <si>
-    <t>RESPUESTA 2</t>
-  </si>
-  <si>
-    <t>TIPO CUENTA</t>
-  </si>
-  <si>
-    <t>SEGUNDA PREGUNTA</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>apurimac</t>
-  </si>
-  <si>
-    <t>chocolate</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Tata..QQ@2</t>
-  </si>
-  <si>
-    <t>yulino44</t>
-  </si>
-  <si>
-    <t>Peru$2023@@</t>
-  </si>
-  <si>
-    <t>jordan2023.</t>
+    <t>PRIMERA PREGUNTA1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,14 +104,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,7 +134,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K2" sqref="K2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,9 +430,10 @@
     <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,39 +447,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -489,46 +494,47 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>7</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>